<commit_message>
added which magnet to use (calcualtion) in 2d-materials-gen.xlsx
</commit_message>
<xml_diff>
--- a/generator/2dparts_schematic_materials-gen.xlsx
+++ b/generator/2dparts_schematic_materials-gen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DFD1D0-0161-48E1-AA11-11AE567D51C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE086BC5-8ACF-43EF-8001-4AF44A9ECAC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6EB7C18F-EE50-4A76-837B-874021D0598F}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="130">
   <si>
     <t>Materials</t>
   </si>
@@ -107,18 +107,9 @@
     <t>total pesos</t>
   </si>
   <si>
-    <t>Magnet calculation</t>
-  </si>
-  <si>
     <t>https://shopee.ph/Ndfeb-Strong-Magnetic-Iron-Steel-Round-Magnet-8X5mm-10mmX2mm-Square-i.695869163.22240112136?sp_atk=20cbdc45-1ba8-420e-a857-3fbb36ea8554&amp;xptdk=20cbdc45-1ba8-420e-a857-3fbb36ea8554</t>
   </si>
   <si>
-    <t>how many to buy?</t>
-  </si>
-  <si>
-    <t>size in mm</t>
-  </si>
-  <si>
     <t>quantity per buy</t>
   </si>
   <si>
@@ -155,9 +146,6 @@
     <t>Part F</t>
   </si>
   <si>
-    <t>volume in mm</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -267,6 +255,168 @@
   </si>
   <si>
     <t>Rotor</t>
+  </si>
+  <si>
+    <t>https://shopee.ph/STRONG-CERAMIC-FERRITE-RECTANGLE-MAGNET-and-ROUND-MAGNET-for-School-Project-and-DIY-Experiment.-i.309964368.21814181743?is_from_login=true</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>option</t>
+  </si>
+  <si>
+    <t>2 pcs 1x1/2x1/4</t>
+  </si>
+  <si>
+    <t>total volume in mm</t>
+  </si>
+  <si>
+    <t>volume size in mm</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>1pc 40x20x8</t>
+  </si>
+  <si>
+    <t>https://shopee.ph/1-Piece-20mm-x-20mm-x-3mm-(-20mm-L-x-20mm-W-x-3mm-H-)-Super-Strong-Neodymium-Rectangular-Bar-Magnet.-i.309964368.6183250145?sp_atk=24622d3e-1718-4baa-88d9-710afd4f766e&amp;xptdk=24622d3e-1718-4baa-88d9-710afd4f766e</t>
+  </si>
+  <si>
+    <t>long end bar</t>
+  </si>
+  <si>
+    <t>pizza bar</t>
+  </si>
+  <si>
+    <t>in mm</t>
+  </si>
+  <si>
+    <t>square 20x2</t>
+  </si>
+  <si>
+    <t>no.</t>
+  </si>
+  <si>
+    <t>for no 1</t>
+  </si>
+  <si>
+    <t>for no 4</t>
+  </si>
+  <si>
+    <t>pizza circle</t>
+  </si>
+  <si>
+    <t>10pcs 30x3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">each piece only has </t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>surface area</t>
+  </si>
+  <si>
+    <t>mm^3</t>
+  </si>
+  <si>
+    <t>mm^2</t>
+  </si>
+  <si>
+    <t>for 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">volume </t>
+  </si>
+  <si>
+    <t>TARGET SURFACE AREA FOR EACH UNIT IN THE STATOR</t>
+  </si>
+  <si>
+    <t>80 MM</t>
+  </si>
+  <si>
+    <t>8 CM</t>
+  </si>
+  <si>
+    <t>(40 x 20)mm</t>
+  </si>
+  <si>
+    <t>(4 x 2)cm</t>
+  </si>
+  <si>
+    <t>as opposed to the target of 80mm surface (see q13)</t>
+  </si>
+  <si>
+    <t>how many to buy (to get the target surface are of stator)</t>
+  </si>
+  <si>
+    <t>STATOR HAS</t>
+  </si>
+  <si>
+    <t>TOTAL UNITS</t>
+  </si>
+  <si>
+    <t>SURFACE AREA (mm) TIMES quantity per buy</t>
+  </si>
+  <si>
+    <t>hence</t>
+  </si>
+  <si>
+    <t>each piece only has x (in mm)</t>
+  </si>
+  <si>
+    <t>Theres 50 of these, hence</t>
+  </si>
+  <si>
+    <t>total area</t>
+  </si>
+  <si>
+    <t>There is 10 of these, hence</t>
+  </si>
+  <si>
+    <t>mm surface area</t>
+  </si>
+  <si>
+    <t>total surface area</t>
+  </si>
+  <si>
+    <t>for number 3</t>
+  </si>
+  <si>
+    <t>neodymium</t>
+  </si>
+  <si>
+    <t>ferrite</t>
+  </si>
+  <si>
+    <t>shape ( + describe the polarity)</t>
+  </si>
+  <si>
+    <t>Legend:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yellow </t>
+  </si>
+  <si>
+    <t>good contenders</t>
+  </si>
+  <si>
+    <t>light orange</t>
+  </si>
+  <si>
+    <t>important parts</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>PART D: ROTOR Magnet calculation</t>
   </si>
 </sst>
 </file>
@@ -320,15 +470,51 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -360,12 +546,157 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -376,9 +707,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -387,10 +715,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -401,12 +725,77 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -426,6 +815,55 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>251799</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>91719</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D6EF464-691B-7267-7C9A-EAD8D7DFA59E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17533620" y="800100"/>
+          <a:ext cx="3917019" cy="3223539"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -574,7 +1012,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="1731409" y="4626013"/>
-          <a:ext cx="25340372" cy="209223"/>
+          <a:ext cx="28055862" cy="209223"/>
           <a:chOff x="1689847" y="1524225"/>
           <a:chExt cx="18606250" cy="232858"/>
         </a:xfrm>
@@ -1144,7 +1582,9 @@
           <a:ext cx="872836" cy="129946"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
-          <a:avLst/>
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 69387"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
@@ -1489,16 +1929,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>831274</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>166255</xdr:rowOff>
+      <xdr:rowOff>166257</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>387928</xdr:colOff>
+      <xdr:colOff>387926</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>195875</xdr:rowOff>
+      <xdr:rowOff>277092</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1513,12 +1953,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="5159863" y="7627883"/>
-          <a:ext cx="4726311" cy="692728"/>
+          <a:off x="7051965" y="7509166"/>
+          <a:ext cx="4807526" cy="1011379"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 30360"/>
+            <a:gd name="adj1" fmla="val 28674"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1551,7 +1991,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>235526</xdr:colOff>
+      <xdr:colOff>13858</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>41565</xdr:rowOff>
     </xdr:from>
@@ -1559,7 +1999,7 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>290947</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>279005</xdr:rowOff>
+      <xdr:rowOff>263238</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1574,12 +2014,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="6711572" y="7530901"/>
-          <a:ext cx="5114240" cy="665021"/>
+          <a:off x="8963893" y="7412184"/>
+          <a:ext cx="5098473" cy="886689"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 29953"/>
+            <a:gd name="adj1" fmla="val 5707"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1733,10 +2173,71 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>221679</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>110838</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>13855</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>346364</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Connector: Elbow 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{341969F7-68A6-1AA1-0DA7-A1F4D95E1DD7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="6761022" y="6179131"/>
+          <a:ext cx="5112326" cy="3505194"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -16396"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2847,10 +3348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046D2DF6-7029-4E01-AB00-EF8208A806E9}">
-  <dimension ref="A2:P11"/>
+  <dimension ref="A2:V37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2858,12 +3359,21 @@
     <col min="2" max="2" width="35.21875" customWidth="1"/>
     <col min="3" max="3" width="11.77734375" customWidth="1"/>
     <col min="4" max="4" width="14.21875" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="11.21875" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" customWidth="1"/>
+    <col min="13" max="13" width="7.88671875" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" customWidth="1"/>
     <col min="15" max="15" width="14.88671875" customWidth="1"/>
+    <col min="16" max="16" width="11.77734375" customWidth="1"/>
+    <col min="17" max="17" width="14.21875" customWidth="1"/>
+    <col min="18" max="18" width="12" customWidth="1"/>
+    <col min="19" max="19" width="11.21875" customWidth="1"/>
+    <col min="20" max="20" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2880,7 +3390,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2894,17 +3404,25 @@
         <v>1</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="J3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-    </row>
-    <row r="4" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="V3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2920,27 +3438,44 @@
       <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="6" t="s">
+      <c r="I4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="L4" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="M4" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="O4" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" s="6" t="s">
+      <c r="P4" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="P4" s="7"/>
-    </row>
-    <row r="5" spans="1:16" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="S4" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="T4" s="44" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2956,32 +3491,49 @@
       <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="7">
-        <f>K5*L5</f>
-        <v>2400</v>
-      </c>
-      <c r="K5" s="7">
+      <c r="I5" s="43">
+        <v>1</v>
+      </c>
+      <c r="J5" s="6">
+        <f>K5*(N5*M5)</f>
+        <v>4800</v>
+      </c>
+      <c r="K5" s="6">
         <f>8*3*2</f>
         <v>48</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="45">
+        <f>3*2*M5</f>
+        <v>300</v>
+      </c>
+      <c r="M5" s="45">
         <v>50</v>
       </c>
-      <c r="M5" s="7">
-        <v>1</v>
-      </c>
-      <c r="N5" s="7">
+      <c r="N5" s="45">
+        <f>IF(M5 &lt;8, 8/M5, IF(ROUND(($T$15)/(L5/10),0.1)=0,1,ROUND(($T$15)/(L5/10),0.1)))</f>
+        <v>2</v>
+      </c>
+      <c r="O5" s="45">
         <v>239</v>
       </c>
-      <c r="O5" s="7">
-        <f>M5*N5</f>
-        <v>239</v>
-      </c>
-      <c r="P5" s="8" t="s">
+      <c r="P5" s="45">
+        <f>N5*O5</f>
+        <v>478</v>
+      </c>
+      <c r="Q5" s="19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="T5" s="45" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2997,32 +3549,49 @@
       <c r="E6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="7">
-        <f>K6*M6</f>
-        <v>2400</v>
-      </c>
-      <c r="K6" s="7">
+      <c r="I6" s="6">
+        <v>2</v>
+      </c>
+      <c r="J6" s="6">
+        <f>K6*(N6*M6)</f>
+        <v>320</v>
+      </c>
+      <c r="K6" s="6">
         <f>20*2</f>
         <v>40</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="45">
+        <f>20*10*M6</f>
+        <v>200</v>
+      </c>
+      <c r="M6" s="45">
         <v>1</v>
       </c>
-      <c r="M6" s="7">
-        <v>60</v>
-      </c>
-      <c r="N6" s="7">
+      <c r="N6" s="45">
+        <f>IF(M6 &lt;8, 8/M6, IF(ROUND(($T$15)/(L6/10),0.1)=0,1,ROUND(($T$15)/(L6/10),0.1)))</f>
+        <v>8</v>
+      </c>
+      <c r="O6" s="45">
         <v>27</v>
       </c>
-      <c r="O6" s="7">
-        <f>M6*N6</f>
-        <v>1620</v>
-      </c>
-      <c r="P6" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P6" s="45">
+        <f>N6*O6</f>
+        <v>216</v>
+      </c>
+      <c r="Q6" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="T6" s="45" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -3038,8 +3607,49 @@
       <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I7" s="6">
+        <v>3</v>
+      </c>
+      <c r="J7" s="6">
+        <f>K7*(N7*M7)</f>
+        <v>163.87063999999998</v>
+      </c>
+      <c r="K7" s="6">
+        <f>(2.54*(2.54/2)*(2.54/4))*10</f>
+        <v>20.483829999999998</v>
+      </c>
+      <c r="L7" s="45">
+        <f>25.4*(25.4/2)*M7</f>
+        <v>645.16</v>
+      </c>
+      <c r="M7" s="45">
+        <v>2</v>
+      </c>
+      <c r="N7" s="45">
+        <f>IF(M7 &lt;8, 8/M7, IF(ROUND(($T$15)/(L7/10),0.1)=0,1,ROUND(($T$15)/(L7/10),0.1)))</f>
+        <v>4</v>
+      </c>
+      <c r="O7" s="45">
+        <v>55</v>
+      </c>
+      <c r="P7" s="45">
+        <f>N7*O7</f>
+        <v>220</v>
+      </c>
+      <c r="Q7" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="T7" s="45" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -3047,16 +3657,57 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="I8" s="43">
+        <v>4</v>
+      </c>
+      <c r="J8" s="6">
+        <f>K8*(N8*M8)</f>
+        <v>21205.750411731104</v>
+      </c>
+      <c r="K8" s="6">
+        <f>(PI()*(15*15))*3</f>
+        <v>2120.5750411731105</v>
+      </c>
+      <c r="L8" s="45">
+        <f>M8*(PI()*15*15)</f>
+        <v>7068.5834705770339</v>
+      </c>
+      <c r="M8" s="45">
+        <v>10</v>
+      </c>
+      <c r="N8" s="45">
+        <f>IF(M8 &lt;8, 8/M8, IF(ROUND(($T$15)/(L8/10),0.1)=0,1,ROUND(($T$15)/(L8/10),0.1)))</f>
+        <v>1</v>
+      </c>
+      <c r="O8" s="45">
+        <v>110</v>
+      </c>
+      <c r="P8" s="45">
+        <f>N8*O8</f>
+        <v>110</v>
+      </c>
+      <c r="Q8" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="S8" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="T8" s="45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -3064,16 +3715,57 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="I9" s="6">
+        <v>5</v>
+      </c>
+      <c r="J9" s="6">
+        <f>K9*(N9*M9)</f>
+        <v>51200</v>
+      </c>
+      <c r="K9" s="6">
+        <f>40*20*8</f>
+        <v>6400</v>
+      </c>
+      <c r="L9" s="45">
+        <f>40*20*M9</f>
+        <v>800</v>
+      </c>
+      <c r="M9" s="45">
+        <v>1</v>
+      </c>
+      <c r="N9" s="45">
+        <f>IF(M9 &lt;8, 8/M9, IF(ROUND(($T$15)/(L9/10),0.1)=0,1,ROUND(($T$15)/(L9/10),0.1)))</f>
+        <v>8</v>
+      </c>
+      <c r="O9" s="45">
+        <v>45</v>
+      </c>
+      <c r="P9" s="45">
+        <f t="shared" ref="P9:P10" si="0">N9*O9</f>
+        <v>360</v>
+      </c>
+      <c r="Q9" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="S9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="T9" s="45" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -3089,13 +3781,54 @@
       <c r="E10" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I10" s="43">
+        <v>6</v>
+      </c>
+      <c r="J10" s="6">
+        <f>K10*(N10*M10)</f>
+        <v>9600</v>
+      </c>
+      <c r="K10" s="6">
+        <f>20*20*3</f>
+        <v>1200</v>
+      </c>
+      <c r="L10" s="45">
+        <f>20*20*M10</f>
+        <v>400</v>
+      </c>
+      <c r="M10" s="45">
+        <v>1</v>
+      </c>
+      <c r="N10" s="45">
+        <f>IF(M10 &lt;8, 8/M10, IF(ROUND(($T$15)/(L10/10),0.1)=0,1,ROUND(($T$15)/(L10/10),0.1)))</f>
+        <v>8</v>
+      </c>
+      <c r="O10" s="45">
+        <v>69</v>
+      </c>
+      <c r="P10" s="45">
+        <f t="shared" si="0"/>
+        <v>552</v>
+      </c>
+      <c r="Q10" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="S10" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="T10" s="45" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -3107,15 +3840,243 @@
         <v>7</v>
       </c>
     </row>
+    <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I13" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" t="s">
+        <v>113</v>
+      </c>
+      <c r="P13" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="35"/>
+      <c r="S13" s="35"/>
+      <c r="T13" s="36"/>
+    </row>
+    <row r="14" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I14" s="18"/>
+      <c r="J14" s="42">
+        <f>3*2</f>
+        <v>6</v>
+      </c>
+      <c r="K14" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="R14" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="S14" s="16"/>
+      <c r="T14" s="28"/>
+    </row>
+    <row r="15" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P15" s="27"/>
+      <c r="Q15" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="R15" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="S15" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="T15" s="33">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J16" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="K16" s="16"/>
+      <c r="P16" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q16" s="31">
+        <v>8</v>
+      </c>
+      <c r="R16" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="S16" s="29"/>
+      <c r="T16" s="22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J17" s="42">
+        <f>6*50</f>
+        <v>300</v>
+      </c>
+      <c r="K17" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+    </row>
+    <row r="18" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="P18" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q18" s="48"/>
+    </row>
+    <row r="19" spans="9:17" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P19" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="P20" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q20" s="46" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="P21" s="49" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q21" s="46"/>
+    </row>
+    <row r="22" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="I22" t="s">
+        <v>92</v>
+      </c>
+      <c r="J22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J23">
+        <f xml:space="preserve"> K8/10</f>
+        <v>212.05750411731105</v>
+      </c>
+      <c r="K23" t="s">
+        <v>96</v>
+      </c>
+      <c r="L23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J24" s="42">
+        <f>J23/3</f>
+        <v>70.685834705770347</v>
+      </c>
+      <c r="K24" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="L24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J27" s="42">
+        <f>J24*10</f>
+        <v>706.85834705770344</v>
+      </c>
+      <c r="K27" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="I31" t="s">
+        <v>100</v>
+      </c>
+      <c r="J31" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="K31" s="21"/>
+    </row>
+    <row r="32" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J32" s="40">
+        <f>20*20</f>
+        <v>400</v>
+      </c>
+      <c r="K32" s="41" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="10:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="10:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J35" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="K35" s="39">
+        <f>20*20</f>
+        <v>400</v>
+      </c>
+      <c r="L35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J36" t="s">
+        <v>50</v>
+      </c>
+      <c r="K36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J37" t="s">
+        <v>101</v>
+      </c>
+      <c r="K37">
+        <f>K35*K36</f>
+        <v>1200</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="J3:P3"/>
+  <mergeCells count="4">
+    <mergeCell ref="P13:T13"/>
+    <mergeCell ref="I3:T3"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="P18:Q18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" display="https://shopee.ph/60m-10m-of-Magnet-Wire-Enameled-Copper-Wire-Winding-For-Making-Electromagnet-Motor-0.1mm-0.2mm-0.3mm-0.4mm-0.5mm-0.6mm-0.7mm-0.8mm-0.9mm-i.866205405.18246963879?sp_atk=ae06ff3a-610c-4cd3-855c-e95fd915dcec&amp;xptdk=ae06ff3a-610c-4cd3-855c-e95fd915dcec" xr:uid="{16CAF327-D6E0-409C-AEC9-9D6A58D245E4}"/>
+    <hyperlink ref="Q6" r:id="rId2" xr:uid="{F1509F84-D5FA-4239-A3F2-CB1AD564F8D0}"/>
+    <hyperlink ref="Q7" r:id="rId3" xr:uid="{11B2DB66-5F7E-4981-8772-FA39308BB3BF}"/>
+    <hyperlink ref="Q10" r:id="rId4" xr:uid="{6C938B4C-A759-4AA6-9A02-15A755BC6434}"/>
+    <hyperlink ref="Q9" r:id="rId5" xr:uid="{FB0FD050-5EA5-4B07-A207-889C4279FA53}"/>
+    <hyperlink ref="Q8" r:id="rId6" xr:uid="{ED6D9EC5-3A94-46C5-B490-2EDA6BBF6564}"/>
+    <hyperlink ref="Q5" r:id="rId7" xr:uid="{586BA7CE-AB65-4085-806A-46D12641CAAD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
+  <drawing r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -3123,13 +4084,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529E1EE1-84BC-44E9-9DB6-5CF40692FF92}">
   <dimension ref="B2:AS54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="E12" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="U54" sqref="U54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="3" max="3" width="36" customWidth="1"/>
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="14" max="14" width="12.77734375" customWidth="1"/>
+    <col min="21" max="21" width="11.88671875" customWidth="1"/>
+    <col min="35" max="35" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
@@ -3140,34 +4106,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:45" s="10" customFormat="1" ht="29.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B30" s="10" t="s">
+    <row r="30" spans="2:45" s="9" customFormat="1" ht="29.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AS30" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="3:35" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C51" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="J51" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI51" s="52" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="3:35" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="K54" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="N54" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="AS30" s="10" t="s">
+      <c r="U54" s="52" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="51" spans="3:35" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C51" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="J51" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI51" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="54" spans="3:35" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="K54" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="N54" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="U54" s="9" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -3180,7 +4146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AEB8265-3C8E-4609-81CC-B5279E8DC9E7}">
   <dimension ref="A2:V44"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
@@ -3198,230 +4164,228 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
+      <c r="D8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="N8" t="s">
+        <v>45</v>
+      </c>
+      <c r="U8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B7" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="D10" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J8" t="s">
-        <v>48</v>
-      </c>
-      <c r="N8" t="s">
-        <v>49</v>
-      </c>
-      <c r="U8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B10" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="M12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="N12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="O12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="R12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B25" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B25" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>52</v>
+      <c r="C25" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B26" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="8" t="s">
+      <c r="B26" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>53</v>
+      <c r="C26" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="M26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="Q26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>53</v>
+      <c r="B27" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
       <c r="O27" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>65</v>
+      </c>
+      <c r="U27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>69</v>
-      </c>
-      <c r="U27" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>71</v>
       </c>
       <c r="E28">
         <v>2</v>
       </c>
-      <c r="M28" s="13"/>
+      <c r="M28" s="10"/>
       <c r="U28" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="7" t="s">
+      <c r="B29" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="17" t="s">
-        <v>34</v>
+      <c r="C29" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="N29" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="V29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="20"/>
-      <c r="N30" s="14"/>
+      <c r="C30" s="3"/>
+      <c r="N30" s="11"/>
       <c r="V30" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="P31" s="13"/>
+      <c r="P31" s="10"/>
       <c r="V31" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="N34" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified 2dschematicgen.xsxslxls (replaced bearings to the magnet stands )and many more
</commit_message>
<xml_diff>
--- a/generator/2dparts_schematic_materials-gen.xlsx
+++ b/generator/2dparts_schematic_materials-gen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE086BC5-8ACF-43EF-8001-4AF44A9ECAC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3F2DD2-2B8B-4486-A407-BC71AF836E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6EB7C18F-EE50-4A76-837B-874021D0598F}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="127">
   <si>
     <t>Materials</t>
   </si>
@@ -212,51 +212,15 @@
     <t>Part A</t>
   </si>
   <si>
-    <t>CopperWire stand</t>
-  </si>
-  <si>
     <t>Main stand</t>
   </si>
   <si>
-    <t>magnet</t>
-  </si>
-  <si>
-    <t>support 1</t>
-  </si>
-  <si>
-    <t>support 2</t>
-  </si>
-  <si>
     <t>(x * y*z ) cm</t>
   </si>
   <si>
-    <t>Material</t>
-  </si>
-  <si>
-    <t>magnet part:</t>
-  </si>
-  <si>
-    <t>with respect to the included diagram in part A:</t>
-  </si>
-  <si>
-    <t>Make the magnet poles like dis:</t>
-  </si>
-  <si>
-    <t>N &lt;- S</t>
-  </si>
-  <si>
-    <t>using around x magnets each</t>
-  </si>
-  <si>
-    <t>(x*y*z ) cm</t>
-  </si>
-  <si>
     <t>quanitty</t>
   </si>
   <si>
-    <t>Rotor</t>
-  </si>
-  <si>
     <t>https://shopee.ph/STRONG-CERAMIC-FERRITE-RECTANGLE-MAGNET-and-ROUND-MAGNET-for-School-Project-and-DIY-Experiment.-i.309964368.21814181743?is_from_login=true</t>
   </si>
   <si>
@@ -417,6 +381,33 @@
   </si>
   <si>
     <t>PART D: ROTOR Magnet calculation</t>
+  </si>
+  <si>
+    <t>https://shopee.ph/MAGNETIC-WIRES-16-AWG-0.052-QUALILINE-PURE-COPPER-BEST-FOR-REWINDING-MOTOR-SOLDERING-DIY-MOTOR-i.76994263.21050805770</t>
+  </si>
+  <si>
+    <t>Stator: 4 coils</t>
+  </si>
+  <si>
+    <t>Stand support</t>
+  </si>
+  <si>
+    <t>stand</t>
+  </si>
+  <si>
+    <t>Rotor: magnets</t>
+  </si>
+  <si>
+    <t>electron flow manager</t>
+  </si>
+  <si>
+    <t>Part G</t>
+  </si>
+  <si>
+    <t>Rod</t>
+  </si>
+  <si>
+    <t>Flywheel</t>
   </si>
 </sst>
 </file>
@@ -514,7 +505,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -538,11 +529,15 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -691,12 +686,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -725,9 +729,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -737,6 +743,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -796,6 +806,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -867,16 +881,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>270163</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>325581</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>81049</xdr:rowOff>
+      <xdr:rowOff>122612</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>536863</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>50570</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>581891</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>41564</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -891,8 +905,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1489363" y="4625340"/>
-          <a:ext cx="266700" cy="3031375"/>
+          <a:off x="5839690" y="4666903"/>
+          <a:ext cx="256310" cy="2994661"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -988,152 +1002,81 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>512209</xdr:colOff>
+      <xdr:colOff>1729816</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>81722</xdr:rowOff>
+      <xdr:rowOff>81721</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>44</xdr:col>
-      <xdr:colOff>83126</xdr:colOff>
+      <xdr:colOff>83127</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>110836</xdr:rowOff>
+      <xdr:rowOff>110835</xdr:rowOff>
     </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="10" name="Group 9">
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28DCA737-7EC6-3CA2-15FF-3F0E1FD08C78}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E45440C-B646-8B2B-BAA6-BA39D8A37F02}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="1731409" y="4626013"/>
-          <a:ext cx="28055862" cy="209223"/>
-          <a:chOff x="1689847" y="1524225"/>
-          <a:chExt cx="18606250" cy="232858"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="16263532" y="-8688504"/>
+          <a:ext cx="209223" cy="26838256"/>
         </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="Rectangle 7">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E45440C-B646-8B2B-BAA6-BA39D8A37F02}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="5400000">
-            <a:off x="11280293" y="-7258722"/>
-            <a:ext cx="232858" cy="17798751"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent2">
-              <a:lumMod val="40000"/>
-              <a:lumOff val="60000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-PH" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="9" name="Isosceles Triangle 8">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{342C0E4C-1AEC-AF40-75E7-B778E5AB4FD4}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="16200000">
-            <a:off x="1990166" y="1237128"/>
-            <a:ext cx="210672" cy="811309"/>
-          </a:xfrm>
-          <a:prstGeom prst="triangle">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent2">
-              <a:lumMod val="40000"/>
-              <a:lumOff val="60000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-PH" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>476352</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>185406</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>13855</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>69273</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>554182</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>13896</xdr:rowOff>
+      <xdr:rowOff>42</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1148,8 +1091,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5962752" y="5098473"/>
-          <a:ext cx="368776" cy="2770950"/>
+          <a:off x="10063697" y="5084619"/>
+          <a:ext cx="368776" cy="2715532"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1214,70 +1157,6 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-PH" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>429490</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>55419</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>235527</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>41564</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="Oval 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56C3B635-A346-7C41-DB3D-02E9D2C5489C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5306290" y="3699164"/>
-          <a:ext cx="1634837" cy="4849091"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:prstDash val="lgDash"/>
-        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -1374,76 +1253,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>407078</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>143436</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>193964</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>96986</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>70902</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>166296</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="Rectangle 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64DD76BC-871C-4A13-F91D-99B1F9143A4F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8941478" y="5047945"/>
-          <a:ext cx="273424" cy="2544387"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-PH" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>581892</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>138544</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>595746</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>221675</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>180108</xdr:rowOff>
+      <xdr:rowOff>69274</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1457,9 +1276,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="-83127" y="5957454"/>
-          <a:ext cx="2563091" cy="13854"/>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="4468094" y="6061365"/>
+          <a:ext cx="2507670" cy="27711"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -1552,79 +1371,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>721392</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>41564</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>83128</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>110839</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>73572</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>178675</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="26" name="Connector: Elbow 25">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{005253A3-68D1-161C-B15E-CAEE638294AE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="17" idx="4"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipV="1">
-          <a:off x="5836347" y="9325781"/>
-          <a:ext cx="872836" cy="129946"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 69387"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="dk1"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="arrow" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>41563</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>4112</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>569844</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>209729</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>387930</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>235527</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1638,13 +1394,13 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="6305729" y="8181160"/>
-          <a:ext cx="2966681" cy="1677066"/>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="4281057" y="9712037"/>
+          <a:ext cx="3546761" cy="304802"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 99984"/>
+            <a:gd name="adj1" fmla="val 50000"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1678,14 +1434,14 @@
     <xdr:from>
       <xdr:col>35</xdr:col>
       <xdr:colOff>207818</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>69273</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>166254</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>39</xdr:col>
-      <xdr:colOff>346364</xdr:colOff>
+      <xdr:colOff>27714</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>235528</xdr:rowOff>
+      <xdr:rowOff>235529</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1700,12 +1456,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="20837236" y="6206837"/>
-          <a:ext cx="4322619" cy="2576946"/>
+          <a:off x="23386473" y="6054435"/>
+          <a:ext cx="4946075" cy="2258296"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj1" fmla="val 81933"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1932,11 +1688,11 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>831274</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>166257</xdr:rowOff>
+      <xdr:rowOff>110838</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>387926</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>221676</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>277092</xdr:rowOff>
     </xdr:to>
@@ -1953,12 +1709,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="7051965" y="7509166"/>
-          <a:ext cx="4807526" cy="1011379"/>
+          <a:off x="7550730" y="7259782"/>
+          <a:ext cx="4862945" cy="1454729"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 28674"/>
+            <a:gd name="adj1" fmla="val 50000"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2176,9 +1932,9 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>221679</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>110838</xdr:rowOff>
+      <xdr:colOff>637309</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>27709</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
@@ -2199,12 +1955,134 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="6761022" y="6179131"/>
-          <a:ext cx="5112326" cy="3505194"/>
+          <a:off x="7322127" y="6435436"/>
+          <a:ext cx="5015346" cy="3089564"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -16396"/>
+            <a:gd name="adj1" fmla="val 19061"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>110839</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>124691</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>166255</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>207819</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Connector: Elbow 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5432DFFE-189D-F5DB-C5D5-33D36E1D2769}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5929748" y="6664036"/>
+          <a:ext cx="23026252" cy="4946074"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 93622"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>55420</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>83129</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>387932</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>110836</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="Connector: Elbow 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38E3FF4C-B477-2FD9-CE1B-E1D4F607FBE5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="16985676" y="7093527"/>
+          <a:ext cx="4544289" cy="332512"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -1524"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2621,16 +2499,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2645,8 +2523,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9525000" y="6355080"/>
-          <a:ext cx="266700" cy="1607820"/>
+          <a:off x="6393180" y="5158740"/>
+          <a:ext cx="266700" cy="1584960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2681,83 +2559,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Rectangle 10">
+        <xdr:cNvPr id="4" name="Rectangle 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99277052-EF46-6A64-845C-A1E7ED274EDB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="9517380" y="5676900"/>
-          <a:ext cx="266700" cy="1607820"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-PH" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>304611</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>97586</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>530246</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>334464</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Rectangle 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{526A55B9-09FF-6C58-9119-07F491E9AB0A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3787A484-EE59-A90C-241A-954494E2DC36}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2765,261 +2583,12 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8831391" y="5797346"/>
-          <a:ext cx="225635" cy="785518"/>
+          <a:off x="7376160" y="5113020"/>
+          <a:ext cx="266700" cy="1584960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-PH" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>487491</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>120446</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>103526</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>357324</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="Rectangle 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC299FB4-0AE2-23C4-FBBC-A5CA4EE98DBC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10233471" y="5820206"/>
-          <a:ext cx="225635" cy="785518"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-PH" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>358140</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="Oval 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EF4316B-CE73-0E20-950F-C27E28E22C0B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9433560" y="6240780"/>
-          <a:ext cx="449580" cy="373380"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-PH" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>320040</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Oval 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5212D3BA-3C1E-EA9F-4FA8-BA8E2EBE7FD3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8679180" y="5654040"/>
-          <a:ext cx="449580" cy="373380"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-PH" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>304800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="Oval 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D681144D-4D35-9C81-5FFF-E5D6E0619520}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10134600" y="5638800"/>
-          <a:ext cx="449580" cy="373380"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -3350,8 +2919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046D2DF6-7029-4E01-AB00-EF8208A806E9}">
   <dimension ref="A2:V37"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3404,22 +2973,22 @@
         <v>1</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="I3" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
+      <c r="I3" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
       <c r="V3" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3438,41 +3007,44 @@
       <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="F4" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="I4" s="6" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="L4" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="M4" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="M4" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="44" t="s">
-        <v>108</v>
-      </c>
-      <c r="O4" s="44" t="s">
+      <c r="N4" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="O4" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="44" t="s">
+      <c r="P4" s="46" t="s">
         <v>25</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="R4" s="17" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="S4" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="T4" s="44" t="s">
-        <v>122</v>
+        <v>71</v>
+      </c>
+      <c r="T4" s="46" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3488,10 +3060,10 @@
       <c r="D5">
         <v>2</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="43">
+      <c r="I5" s="45">
         <v>1</v>
       </c>
       <c r="J5" s="6">
@@ -3502,21 +3074,21 @@
         <f>8*3*2</f>
         <v>48</v>
       </c>
-      <c r="L5" s="45">
+      <c r="L5" s="47">
         <f>3*2*M5</f>
         <v>300</v>
       </c>
-      <c r="M5" s="45">
+      <c r="M5" s="47">
         <v>50</v>
       </c>
-      <c r="N5" s="45">
+      <c r="N5" s="47">
         <f>IF(M5 &lt;8, 8/M5, IF(ROUND(($T$15)/(L5/10),0.1)=0,1,ROUND(($T$15)/(L5/10),0.1)))</f>
         <v>2</v>
       </c>
-      <c r="O5" s="45">
+      <c r="O5" s="47">
         <v>239</v>
       </c>
-      <c r="P5" s="45">
+      <c r="P5" s="47">
         <f>N5*O5</f>
         <v>478</v>
       </c>
@@ -3527,10 +3099,10 @@
         <v>30</v>
       </c>
       <c r="S5" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="T5" s="45" t="s">
-        <v>86</v>
+        <v>108</v>
+      </c>
+      <c r="T5" s="47" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3546,7 +3118,7 @@
       <c r="D6">
         <v>50</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I6" s="6">
@@ -3560,21 +3132,21 @@
         <f>20*2</f>
         <v>40</v>
       </c>
-      <c r="L6" s="45">
+      <c r="L6" s="47">
         <f>20*10*M6</f>
         <v>200</v>
       </c>
-      <c r="M6" s="45">
+      <c r="M6" s="47">
         <v>1</v>
       </c>
-      <c r="N6" s="45">
+      <c r="N6" s="47">
         <f>IF(M6 &lt;8, 8/M6, IF(ROUND(($T$15)/(L6/10),0.1)=0,1,ROUND(($T$15)/(L6/10),0.1)))</f>
         <v>8</v>
       </c>
-      <c r="O6" s="45">
+      <c r="O6" s="47">
         <v>27</v>
       </c>
-      <c r="P6" s="45">
+      <c r="P6" s="47">
         <f>N6*O6</f>
         <v>216</v>
       </c>
@@ -3582,13 +3154,13 @@
         <v>26</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="T6" s="45" t="s">
-        <v>86</v>
+        <v>108</v>
+      </c>
+      <c r="T6" s="47" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
@@ -3618,35 +3190,35 @@
         <f>(2.54*(2.54/2)*(2.54/4))*10</f>
         <v>20.483829999999998</v>
       </c>
-      <c r="L7" s="45">
+      <c r="L7" s="47">
         <f>25.4*(25.4/2)*M7</f>
         <v>645.16</v>
       </c>
-      <c r="M7" s="45">
+      <c r="M7" s="47">
         <v>2</v>
       </c>
-      <c r="N7" s="45">
+      <c r="N7" s="47">
         <f>IF(M7 &lt;8, 8/M7, IF(ROUND(($T$15)/(L7/10),0.1)=0,1,ROUND(($T$15)/(L7/10),0.1)))</f>
         <v>4</v>
       </c>
-      <c r="O7" s="45">
+      <c r="O7" s="47">
         <v>55</v>
       </c>
-      <c r="P7" s="45">
+      <c r="P7" s="47">
         <f>N7*O7</f>
         <v>220</v>
       </c>
-      <c r="Q7" s="32" t="s">
-        <v>76</v>
+      <c r="Q7" s="34" t="s">
+        <v>64</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="T7" s="45" t="s">
-        <v>87</v>
+        <v>109</v>
+      </c>
+      <c r="T7" s="47" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
@@ -3665,7 +3237,7 @@
       <c r="E8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="43">
+      <c r="I8" s="45">
         <v>4</v>
       </c>
       <c r="J8" s="6">
@@ -3676,35 +3248,35 @@
         <f>(PI()*(15*15))*3</f>
         <v>2120.5750411731105</v>
       </c>
-      <c r="L8" s="45">
+      <c r="L8" s="47">
         <f>M8*(PI()*15*15)</f>
         <v>7068.5834705770339</v>
       </c>
-      <c r="M8" s="45">
+      <c r="M8" s="47">
         <v>10</v>
       </c>
-      <c r="N8" s="45">
+      <c r="N8" s="47">
         <f>IF(M8 &lt;8, 8/M8, IF(ROUND(($T$15)/(L8/10),0.1)=0,1,ROUND(($T$15)/(L8/10),0.1)))</f>
         <v>1</v>
       </c>
-      <c r="O8" s="45">
+      <c r="O8" s="47">
         <v>110</v>
       </c>
-      <c r="P8" s="45">
+      <c r="P8" s="47">
         <f>N8*O8</f>
         <v>110</v>
       </c>
-      <c r="Q8" s="32" t="s">
-        <v>76</v>
+      <c r="Q8" s="34" t="s">
+        <v>64</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="T8" s="45" t="s">
-        <v>93</v>
+        <v>109</v>
+      </c>
+      <c r="T8" s="47" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
@@ -3734,35 +3306,35 @@
         <f>40*20*8</f>
         <v>6400</v>
       </c>
-      <c r="L9" s="45">
+      <c r="L9" s="47">
         <f>40*20*M9</f>
         <v>800</v>
       </c>
-      <c r="M9" s="45">
+      <c r="M9" s="47">
         <v>1</v>
       </c>
-      <c r="N9" s="45">
+      <c r="N9" s="47">
         <f>IF(M9 &lt;8, 8/M9, IF(ROUND(($T$15)/(L9/10),0.1)=0,1,ROUND(($T$15)/(L9/10),0.1)))</f>
         <v>8</v>
       </c>
-      <c r="O9" s="45">
+      <c r="O9" s="47">
         <v>45</v>
       </c>
-      <c r="P9" s="45">
+      <c r="P9" s="47">
         <f t="shared" ref="P9:P10" si="0">N9*O9</f>
         <v>360</v>
       </c>
-      <c r="Q9" s="32" t="s">
-        <v>76</v>
+      <c r="Q9" s="34" t="s">
+        <v>64</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="S9" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="T9" s="45" t="s">
-        <v>87</v>
+        <v>109</v>
+      </c>
+      <c r="T9" s="47" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
@@ -3781,7 +3353,7 @@
       <c r="E10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="43">
+      <c r="I10" s="45">
         <v>6</v>
       </c>
       <c r="J10" s="6">
@@ -3792,35 +3364,35 @@
         <f>20*20*3</f>
         <v>1200</v>
       </c>
-      <c r="L10" s="45">
+      <c r="L10" s="47">
         <f>20*20*M10</f>
         <v>400</v>
       </c>
-      <c r="M10" s="45">
+      <c r="M10" s="47">
         <v>1</v>
       </c>
-      <c r="N10" s="45">
+      <c r="N10" s="47">
         <f>IF(M10 &lt;8, 8/M10, IF(ROUND(($T$15)/(L10/10),0.1)=0,1,ROUND(($T$15)/(L10/10),0.1)))</f>
         <v>8</v>
       </c>
-      <c r="O10" s="45">
+      <c r="O10" s="47">
         <v>69</v>
       </c>
-      <c r="P10" s="45">
+      <c r="P10" s="47">
         <f t="shared" si="0"/>
         <v>552</v>
       </c>
-      <c r="Q10" s="32" t="s">
-        <v>85</v>
+      <c r="Q10" s="34" t="s">
+        <v>73</v>
       </c>
       <c r="R10" s="6" t="s">
         <v>30</v>
       </c>
       <c r="S10" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="T10" s="45" t="s">
-        <v>87</v>
+        <v>108</v>
+      </c>
+      <c r="T10" s="47" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
@@ -3843,82 +3415,82 @@
     <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I13" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="J13" t="s">
-        <v>113</v>
-      </c>
-      <c r="P13" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="35"/>
-      <c r="S13" s="35"/>
-      <c r="T13" s="36"/>
+        <v>101</v>
+      </c>
+      <c r="P13" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="38"/>
     </row>
     <row r="14" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I14" s="18"/>
-      <c r="J14" s="42">
+      <c r="J14" s="44">
         <f>3*2</f>
         <v>6</v>
       </c>
-      <c r="K14" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="R14" s="24" t="s">
+      <c r="K14" s="41" t="s">
         <v>105</v>
       </c>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="R14" s="26" t="s">
+        <v>93</v>
+      </c>
       <c r="S14" s="16"/>
-      <c r="T14" s="28"/>
+      <c r="T14" s="30"/>
     </row>
     <row r="15" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="P15" s="27"/>
-      <c r="Q15" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="R15" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="S15" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="T15" s="33">
+      <c r="P15" s="29"/>
+      <c r="Q15" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="R15" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="S15" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="T15" s="35">
         <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J16" s="37" t="s">
-        <v>114</v>
+      <c r="J16" s="39" t="s">
+        <v>102</v>
       </c>
       <c r="K16" s="16"/>
-      <c r="P16" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q16" s="31">
+      <c r="P16" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q16" s="33">
         <v>8</v>
       </c>
-      <c r="R16" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="S16" s="29"/>
-      <c r="T16" s="22" t="s">
-        <v>82</v>
+      <c r="R16" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="S16" s="31"/>
+      <c r="T16" s="24" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J17" s="42">
+      <c r="J17" s="44">
         <f>6*50</f>
         <v>300</v>
       </c>
-      <c r="K17" s="39" t="s">
-        <v>115</v>
+      <c r="K17" s="41" t="s">
+        <v>103</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="M17" s="16"/>
       <c r="N17" s="16"/>
@@ -3926,39 +3498,39 @@
     <row r="18" spans="9:17" x14ac:dyDescent="0.3">
       <c r="M18" s="16"/>
       <c r="N18" s="16"/>
-      <c r="P18" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q18" s="48"/>
+      <c r="P18" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q18" s="50"/>
     </row>
     <row r="19" spans="9:17" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="P19" s="50" t="s">
-        <v>124</v>
+      <c r="P19" s="52" t="s">
+        <v>112</v>
       </c>
       <c r="Q19" s="7" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="9:17" x14ac:dyDescent="0.3">
-      <c r="P20" s="51" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q20" s="46" t="s">
-        <v>127</v>
+      <c r="P20" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q20" s="48" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="9:17" x14ac:dyDescent="0.3">
-      <c r="P21" s="49" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q21" s="46"/>
+      <c r="P21" s="51" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q21" s="48"/>
     </row>
     <row r="22" spans="9:17" x14ac:dyDescent="0.3">
       <c r="I22" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="J22" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3967,78 +3539,78 @@
         <v>212.05750411731105</v>
       </c>
       <c r="K23" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="L23" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J24" s="42">
+      <c r="J24" s="44">
         <f>J23/3</f>
         <v>70.685834705770347</v>
       </c>
-      <c r="K24" s="39" t="s">
-        <v>97</v>
+      <c r="K24" s="41" t="s">
+        <v>85</v>
       </c>
       <c r="L24" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="M24" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J26" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J27" s="42">
+      <c r="J27" s="44">
         <f>J24*10</f>
         <v>706.85834705770344</v>
       </c>
-      <c r="K27" s="39" t="s">
-        <v>115</v>
+      <c r="K27" s="41" t="s">
+        <v>103</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="31" spans="9:17" x14ac:dyDescent="0.3">
       <c r="I31" t="s">
-        <v>100</v>
-      </c>
-      <c r="J31" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="K31" s="21"/>
+        <v>88</v>
+      </c>
+      <c r="J31" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="K31" s="23"/>
     </row>
     <row r="32" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J32" s="40">
+      <c r="J32" s="42">
         <f>20*20</f>
         <v>400</v>
       </c>
-      <c r="K32" s="41" t="s">
-        <v>97</v>
+      <c r="K32" s="43" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="10:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J34" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="10:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J35" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="K35" s="39">
+      <c r="J35" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="K35" s="41">
         <f>20*20</f>
         <v>400</v>
       </c>
       <c r="L35" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="10:12" x14ac:dyDescent="0.3">
@@ -4051,7 +3623,7 @@
     </row>
     <row r="37" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J37" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="K37">
         <f>K35*K36</f>
@@ -4073,29 +3645,34 @@
     <hyperlink ref="Q9" r:id="rId5" xr:uid="{FB0FD050-5EA5-4B07-A207-889C4279FA53}"/>
     <hyperlink ref="Q8" r:id="rId6" xr:uid="{ED6D9EC5-3A94-46C5-B490-2EDA6BBF6564}"/>
     <hyperlink ref="Q5" r:id="rId7" xr:uid="{586BA7CE-AB65-4085-806A-46D12641CAAD}"/>
+    <hyperlink ref="F4" r:id="rId8" xr:uid="{24937DAD-138E-480B-8C9B-C41A63910301}"/>
+    <hyperlink ref="E5" r:id="rId9" xr:uid="{9AE1FFA3-BCB6-4847-A6FB-584E874F1FEC}"/>
+    <hyperlink ref="E6" r:id="rId10" xr:uid="{D4B491E7-7194-451B-A1B0-1976E030619D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
-  <drawing r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
+  <drawing r:id="rId12"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529E1EE1-84BC-44E9-9DB6-5CF40692FF92}">
-  <dimension ref="B2:AS54"/>
+  <dimension ref="B2:AS60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E12" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="U54" sqref="U54"/>
+    <sheetView tabSelected="1" topLeftCell="F15" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AA54" sqref="AA54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="36" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
     <col min="11" max="11" width="12.33203125" customWidth="1"/>
     <col min="14" max="14" width="12.77734375" customWidth="1"/>
     <col min="21" max="21" width="11.88671875" customWidth="1"/>
-    <col min="35" max="35" width="11.109375" customWidth="1"/>
+    <col min="26" max="26" width="11.109375" customWidth="1"/>
+    <col min="35" max="35" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
@@ -4106,8 +3683,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:45" s="9" customFormat="1" ht="29.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B30" s="9" t="s">
+    <row r="30" spans="6:45" s="9" customFormat="1" ht="29.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="F30" s="9" t="s">
         <v>31</v>
       </c>
       <c r="AS30" s="9" t="s">
@@ -4115,25 +3692,30 @@
       </c>
     </row>
     <row r="51" spans="3:35" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C51" s="52" t="s">
+      <c r="C51" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="J51" s="52" t="s">
+      <c r="Z51" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI51" s="54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="3:35" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="K54" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="N54" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="U54" s="54" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="3:35" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="F60" s="54" t="s">
         <v>37</v>
-      </c>
-      <c r="AI51" s="52" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="54" spans="3:35" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="K54" s="52" t="s">
-        <v>35</v>
-      </c>
-      <c r="N54" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="U54" s="52" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -4144,10 +3726,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AEB8265-3C8E-4609-81CC-B5279E8DC9E7}">
-  <dimension ref="A2:V44"/>
+  <dimension ref="A2:U63"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4259,15 +3841,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="12" t="s">
         <v>40</v>
       </c>
@@ -4277,115 +3859,91 @@
       <c r="D25" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B26" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="7" t="s">
+      <c r="E25" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B26" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="C26" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="6">
         <v>1</v>
       </c>
-      <c r="M26" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="O27" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>65</v>
-      </c>
-      <c r="U27" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
+      <c r="I26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="55"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+    </row>
+    <row r="28" spans="1:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="16"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
       <c r="M28" s="10"/>
-      <c r="U28" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="N29" t="s">
-        <v>64</v>
-      </c>
-      <c r="V29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="16"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+    </row>
+    <row r="30" spans="1:16" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="3"/>
       <c r="N30" s="11"/>
-      <c r="V30" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="P31" s="10"/>
-      <c r="V31" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="N34" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>75</v>
+      <c r="B37" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aslkdjalskd update shape of magnet candidate 2
</commit_message>
<xml_diff>
--- a/generator/2dparts_schematic_materials-gen.xlsx
+++ b/generator/2dparts_schematic_materials-gen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3F2DD2-2B8B-4486-A407-BC71AF836E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BF4BBD-EA21-43D2-B9BF-62F20F527D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6EB7C18F-EE50-4A76-837B-874021D0598F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6EB7C18F-EE50-4A76-837B-874021D0598F}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
@@ -700,7 +700,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -729,16 +729,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -765,16 +755,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -787,15 +767,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -809,6 +780,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2919,8 +2911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046D2DF6-7029-4E01-AB00-EF8208A806E9}">
   <dimension ref="A2:V37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2973,20 +2965,20 @@
         <v>1</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
       <c r="V3" t="s">
         <v>107</v>
       </c>
@@ -3019,31 +3011,31 @@
       <c r="K4" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="46" t="s">
+      <c r="L4" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="M4" s="46" t="s">
+      <c r="M4" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="46" t="s">
+      <c r="N4" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="O4" s="46" t="s">
+      <c r="O4" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="46" t="s">
+      <c r="P4" s="38" t="s">
         <v>25</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="R4" s="17" t="s">
+      <c r="R4" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="S4" s="17" t="s">
+      <c r="S4" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="T4" s="46" t="s">
+      <c r="T4" s="38" t="s">
         <v>110</v>
       </c>
     </row>
@@ -3063,36 +3055,36 @@
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="45">
+      <c r="I5" s="37">
         <v>1</v>
       </c>
       <c r="J5" s="6">
-        <f>K5*(N5*M5)</f>
+        <f t="shared" ref="J5:J10" si="0">K5*(N5*M5)</f>
         <v>4800</v>
       </c>
       <c r="K5" s="6">
         <f>8*3*2</f>
         <v>48</v>
       </c>
-      <c r="L5" s="47">
+      <c r="L5" s="39">
         <f>3*2*M5</f>
         <v>300</v>
       </c>
-      <c r="M5" s="47">
+      <c r="M5" s="39">
         <v>50</v>
       </c>
-      <c r="N5" s="47">
-        <f>IF(M5 &lt;8, 8/M5, IF(ROUND(($T$15)/(L5/10),0.1)=0,1,ROUND(($T$15)/(L5/10),0.1)))</f>
+      <c r="N5" s="39">
+        <f t="shared" ref="N5:N10" si="1">IF(M5 &lt;8, 8/M5, IF(ROUND(($T$15)/(L5/10),0.1)=0,1,ROUND(($T$15)/(L5/10),0.1)))</f>
         <v>2</v>
       </c>
-      <c r="O5" s="47">
+      <c r="O5" s="39">
         <v>239</v>
       </c>
-      <c r="P5" s="47">
+      <c r="P5" s="39">
         <f>N5*O5</f>
         <v>478</v>
       </c>
-      <c r="Q5" s="19" t="s">
+      <c r="Q5" s="15" t="s">
         <v>24</v>
       </c>
       <c r="R5" s="6" t="s">
@@ -3101,7 +3093,7 @@
       <c r="S5" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="T5" s="47" t="s">
+      <c r="T5" s="39" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3125,32 +3117,32 @@
         <v>2</v>
       </c>
       <c r="J6" s="6">
-        <f>K6*(N6*M6)</f>
+        <f t="shared" si="0"/>
         <v>320</v>
       </c>
       <c r="K6" s="6">
         <f>20*2</f>
         <v>40</v>
       </c>
-      <c r="L6" s="47">
+      <c r="L6" s="39">
         <f>20*10*M6</f>
         <v>200</v>
       </c>
-      <c r="M6" s="47">
+      <c r="M6" s="39">
         <v>1</v>
       </c>
-      <c r="N6" s="47">
-        <f>IF(M6 &lt;8, 8/M6, IF(ROUND(($T$15)/(L6/10),0.1)=0,1,ROUND(($T$15)/(L6/10),0.1)))</f>
+      <c r="N6" s="39">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="O6" s="47">
+      <c r="O6" s="39">
         <v>27</v>
       </c>
-      <c r="P6" s="47">
+      <c r="P6" s="39">
         <f>N6*O6</f>
         <v>216</v>
       </c>
-      <c r="Q6" s="19" t="s">
+      <c r="Q6" s="15" t="s">
         <v>26</v>
       </c>
       <c r="R6" s="6" t="s">
@@ -3159,8 +3151,8 @@
       <c r="S6" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="T6" s="47" t="s">
-        <v>74</v>
+      <c r="T6" s="39" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
@@ -3183,32 +3175,32 @@
         <v>3</v>
       </c>
       <c r="J7" s="6">
-        <f>K7*(N7*M7)</f>
+        <f t="shared" si="0"/>
         <v>163.87063999999998</v>
       </c>
       <c r="K7" s="6">
         <f>(2.54*(2.54/2)*(2.54/4))*10</f>
         <v>20.483829999999998</v>
       </c>
-      <c r="L7" s="47">
+      <c r="L7" s="39">
         <f>25.4*(25.4/2)*M7</f>
         <v>645.16</v>
       </c>
-      <c r="M7" s="47">
+      <c r="M7" s="39">
         <v>2</v>
       </c>
-      <c r="N7" s="47">
-        <f>IF(M7 &lt;8, 8/M7, IF(ROUND(($T$15)/(L7/10),0.1)=0,1,ROUND(($T$15)/(L7/10),0.1)))</f>
+      <c r="N7" s="39">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="O7" s="47">
+      <c r="O7" s="39">
         <v>55</v>
       </c>
-      <c r="P7" s="47">
+      <c r="P7" s="39">
         <f>N7*O7</f>
         <v>220</v>
       </c>
-      <c r="Q7" s="34" t="s">
+      <c r="Q7" s="30" t="s">
         <v>64</v>
       </c>
       <c r="R7" s="6" t="s">
@@ -3217,7 +3209,7 @@
       <c r="S7" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="T7" s="47" t="s">
+      <c r="T7" s="39" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3237,36 +3229,36 @@
       <c r="E8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="45">
+      <c r="I8" s="37">
         <v>4</v>
       </c>
       <c r="J8" s="6">
-        <f>K8*(N8*M8)</f>
+        <f t="shared" si="0"/>
         <v>21205.750411731104</v>
       </c>
       <c r="K8" s="6">
         <f>(PI()*(15*15))*3</f>
         <v>2120.5750411731105</v>
       </c>
-      <c r="L8" s="47">
+      <c r="L8" s="39">
         <f>M8*(PI()*15*15)</f>
         <v>7068.5834705770339</v>
       </c>
-      <c r="M8" s="47">
+      <c r="M8" s="39">
         <v>10</v>
       </c>
-      <c r="N8" s="47">
-        <f>IF(M8 &lt;8, 8/M8, IF(ROUND(($T$15)/(L8/10),0.1)=0,1,ROUND(($T$15)/(L8/10),0.1)))</f>
+      <c r="N8" s="39">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="O8" s="47">
+      <c r="O8" s="39">
         <v>110</v>
       </c>
-      <c r="P8" s="47">
+      <c r="P8" s="39">
         <f>N8*O8</f>
         <v>110</v>
       </c>
-      <c r="Q8" s="34" t="s">
+      <c r="Q8" s="30" t="s">
         <v>64</v>
       </c>
       <c r="R8" s="6" t="s">
@@ -3275,7 +3267,7 @@
       <c r="S8" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="T8" s="47" t="s">
+      <c r="T8" s="39" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3299,32 +3291,32 @@
         <v>5</v>
       </c>
       <c r="J9" s="6">
-        <f>K9*(N9*M9)</f>
+        <f t="shared" si="0"/>
         <v>51200</v>
       </c>
       <c r="K9" s="6">
         <f>40*20*8</f>
         <v>6400</v>
       </c>
-      <c r="L9" s="47">
+      <c r="L9" s="39">
         <f>40*20*M9</f>
         <v>800</v>
       </c>
-      <c r="M9" s="47">
+      <c r="M9" s="39">
         <v>1</v>
       </c>
-      <c r="N9" s="47">
-        <f>IF(M9 &lt;8, 8/M9, IF(ROUND(($T$15)/(L9/10),0.1)=0,1,ROUND(($T$15)/(L9/10),0.1)))</f>
+      <c r="N9" s="39">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="O9" s="47">
+      <c r="O9" s="39">
         <v>45</v>
       </c>
-      <c r="P9" s="47">
-        <f t="shared" ref="P9:P10" si="0">N9*O9</f>
+      <c r="P9" s="39">
+        <f t="shared" ref="P9:P10" si="2">N9*O9</f>
         <v>360</v>
       </c>
-      <c r="Q9" s="34" t="s">
+      <c r="Q9" s="30" t="s">
         <v>64</v>
       </c>
       <c r="R9" s="6" t="s">
@@ -3333,7 +3325,7 @@
       <c r="S9" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="T9" s="47" t="s">
+      <c r="T9" s="39" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3353,36 +3345,36 @@
       <c r="E10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="45">
+      <c r="I10" s="37">
         <v>6</v>
       </c>
       <c r="J10" s="6">
-        <f>K10*(N10*M10)</f>
+        <f t="shared" si="0"/>
         <v>9600</v>
       </c>
       <c r="K10" s="6">
         <f>20*20*3</f>
         <v>1200</v>
       </c>
-      <c r="L10" s="47">
+      <c r="L10" s="39">
         <f>20*20*M10</f>
         <v>400</v>
       </c>
-      <c r="M10" s="47">
+      <c r="M10" s="39">
         <v>1</v>
       </c>
-      <c r="N10" s="47">
-        <f>IF(M10 &lt;8, 8/M10, IF(ROUND(($T$15)/(L10/10),0.1)=0,1,ROUND(($T$15)/(L10/10),0.1)))</f>
+      <c r="N10" s="39">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="O10" s="47">
+      <c r="O10" s="39">
         <v>69</v>
       </c>
-      <c r="P10" s="47">
-        <f t="shared" si="0"/>
+      <c r="P10" s="39">
+        <f t="shared" si="2"/>
         <v>552</v>
       </c>
-      <c r="Q10" s="34" t="s">
+      <c r="Q10" s="30" t="s">
         <v>73</v>
       </c>
       <c r="R10" s="6" t="s">
@@ -3391,7 +3383,7 @@
       <c r="S10" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="T10" s="47" t="s">
+      <c r="T10" s="39" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3420,91 +3412,85 @@
       <c r="J13" t="s">
         <v>101</v>
       </c>
-      <c r="P13" s="36" t="s">
+      <c r="P13" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="37"/>
-      <c r="S13" s="37"/>
-      <c r="T13" s="38"/>
+      <c r="Q13" s="47"/>
+      <c r="R13" s="47"/>
+      <c r="S13" s="47"/>
+      <c r="T13" s="48"/>
     </row>
     <row r="14" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I14" s="18"/>
-      <c r="J14" s="44">
+      <c r="I14" s="14"/>
+      <c r="J14" s="36">
         <f>3*2</f>
         <v>6</v>
       </c>
-      <c r="K14" s="41" t="s">
+      <c r="K14" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="25" t="s">
+      <c r="P14" s="25"/>
+      <c r="Q14" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="R14" s="26" t="s">
+      <c r="R14" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="S14" s="16"/>
-      <c r="T14" s="30"/>
+      <c r="T14" s="26"/>
     </row>
     <row r="15" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="P15" s="29"/>
-      <c r="Q15" s="27" t="s">
+      <c r="P15" s="25"/>
+      <c r="Q15" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="R15" s="28" t="s">
+      <c r="R15" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="S15" s="31" t="s">
+      <c r="S15" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="T15" s="35">
+      <c r="T15" s="31">
         <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J16" s="39" t="s">
+      <c r="J16" t="s">
         <v>102</v>
       </c>
-      <c r="K16" s="16"/>
-      <c r="P16" s="32" t="s">
+      <c r="P16" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="Q16" s="33">
+      <c r="Q16" s="29">
         <v>8</v>
       </c>
-      <c r="R16" s="24" t="s">
+      <c r="R16" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="S16" s="31"/>
-      <c r="T16" s="24" t="s">
+      <c r="S16" s="27"/>
+      <c r="T16" s="20" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="17" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J17" s="44">
+      <c r="J17" s="36">
         <f>6*50</f>
         <v>300</v>
       </c>
-      <c r="K17" s="41" t="s">
+      <c r="K17" s="33" t="s">
         <v>103</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
     </row>
     <row r="18" spans="9:17" x14ac:dyDescent="0.3">
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="P18" s="49" t="s">
+      <c r="P18" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="Q18" s="50"/>
+      <c r="Q18" s="52"/>
     </row>
     <row r="19" spans="9:17" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="P19" s="52" t="s">
+      <c r="P19" s="41" t="s">
         <v>112</v>
       </c>
       <c r="Q19" s="7" t="s">
@@ -3512,18 +3498,18 @@
       </c>
     </row>
     <row r="20" spans="9:17" x14ac:dyDescent="0.3">
-      <c r="P20" s="53" t="s">
+      <c r="P20" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="Q20" s="48" t="s">
+      <c r="Q20" s="50" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="21" spans="9:17" x14ac:dyDescent="0.3">
-      <c r="P21" s="51" t="s">
+      <c r="P21" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="Q21" s="48"/>
+      <c r="Q21" s="50"/>
     </row>
     <row r="22" spans="9:17" x14ac:dyDescent="0.3">
       <c r="I22" t="s">
@@ -3546,11 +3532,11 @@
       </c>
     </row>
     <row r="24" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J24" s="44">
+      <c r="J24" s="36">
         <f>J23/3</f>
         <v>70.685834705770347</v>
       </c>
-      <c r="K24" s="41" t="s">
+      <c r="K24" s="33" t="s">
         <v>85</v>
       </c>
       <c r="L24" t="s">
@@ -3566,11 +3552,11 @@
       </c>
     </row>
     <row r="27" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J27" s="44">
+      <c r="J27" s="36">
         <f>J24*10</f>
         <v>706.85834705770344</v>
       </c>
-      <c r="K27" s="41" t="s">
+      <c r="K27" s="33" t="s">
         <v>103</v>
       </c>
       <c r="L27" s="1" t="s">
@@ -3582,17 +3568,17 @@
       <c r="I31" t="s">
         <v>88</v>
       </c>
-      <c r="J31" s="22" t="s">
+      <c r="J31" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="K31" s="23"/>
+      <c r="K31" s="19"/>
     </row>
     <row r="32" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J32" s="42">
+      <c r="J32" s="34">
         <f>20*20</f>
         <v>400</v>
       </c>
-      <c r="K32" s="43" t="s">
+      <c r="K32" s="35" t="s">
         <v>85</v>
       </c>
     </row>
@@ -3602,10 +3588,10 @@
       </c>
     </row>
     <row r="35" spans="10:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J35" s="40" t="s">
+      <c r="J35" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="K35" s="41">
+      <c r="K35" s="33">
         <f>20*20</f>
         <v>400</v>
       </c>
@@ -3659,7 +3645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529E1EE1-84BC-44E9-9DB6-5CF40692FF92}">
   <dimension ref="B2:AS60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F15" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="F15" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="AA54" sqref="AA54"/>
     </sheetView>
   </sheetViews>
@@ -3692,29 +3678,29 @@
       </c>
     </row>
     <row r="51" spans="3:35" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C51" s="54" t="s">
+      <c r="C51" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="Z51" s="54" t="s">
+      <c r="Z51" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="AI51" s="54" t="s">
+      <c r="AI51" s="43" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="54" spans="3:35" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="K54" s="54" t="s">
+      <c r="K54" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="N54" s="54" t="s">
+      <c r="N54" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="U54" s="54" t="s">
+      <c r="U54" s="43" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="60" spans="3:35" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="F60" s="54" t="s">
+      <c r="F60" s="43" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3864,13 +3850,13 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="17" t="s">
         <v>49</v>
       </c>
       <c r="E26" s="6">
@@ -3881,23 +3867,17 @@
       </c>
     </row>
     <row r="27" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="55"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
     </row>
     <row r="28" spans="1:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="16"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
+      <c r="C28" s="3"/>
       <c r="M28" s="10"/>
     </row>
     <row r="29" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="16"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
+      <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:16" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="3"/>

</xml_diff>

<commit_message>
added ambagan + replaced magnet candidate 1 as pizza bar
</commit_message>
<xml_diff>
--- a/generator/2dparts_schematic_materials-gen.xlsx
+++ b/generator/2dparts_schematic_materials-gen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BF4BBD-EA21-43D2-B9BF-62F20F527D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0041DEC9-985E-4F9A-89A3-7AEFBFA63E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6EB7C18F-EE50-4A76-837B-874021D0598F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6EB7C18F-EE50-4A76-837B-874021D0598F}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="126">
   <si>
     <t>Materials</t>
   </si>
@@ -249,9 +249,6 @@
   </si>
   <si>
     <t>https://shopee.ph/1-Piece-20mm-x-20mm-x-3mm-(-20mm-L-x-20mm-W-x-3mm-H-)-Super-Strong-Neodymium-Rectangular-Bar-Magnet.-i.309964368.6183250145?sp_atk=24622d3e-1718-4baa-88d9-710afd4f766e&amp;xptdk=24622d3e-1718-4baa-88d9-710afd4f766e</t>
-  </si>
-  <si>
-    <t>long end bar</t>
   </si>
   <si>
     <t>pizza bar</t>
@@ -2911,8 +2908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046D2DF6-7029-4E01-AB00-EF8208A806E9}">
   <dimension ref="A2:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2966,7 +2963,7 @@
       </c>
       <c r="E3" s="3"/>
       <c r="I3" s="49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J3" s="49"/>
       <c r="K3" s="49"/>
@@ -2980,7 +2977,7 @@
       <c r="S3" s="49"/>
       <c r="T3" s="49"/>
       <c r="V3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3000,10 +2997,10 @@
         <v>15</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>68</v>
@@ -3012,13 +3009,13 @@
         <v>69</v>
       </c>
       <c r="L4" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M4" s="38" t="s">
         <v>27</v>
       </c>
       <c r="N4" s="38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O4" s="38" t="s">
         <v>28</v>
@@ -3036,7 +3033,7 @@
         <v>71</v>
       </c>
       <c r="T4" s="38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3091,7 +3088,7 @@
         <v>30</v>
       </c>
       <c r="S5" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T5" s="39" t="s">
         <v>74</v>
@@ -3146,13 +3143,13 @@
         <v>26</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T6" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
@@ -3207,10 +3204,10 @@
         <v>67</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T7" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
@@ -3262,13 +3259,13 @@
         <v>64</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T8" s="39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
@@ -3323,10 +3320,10 @@
         <v>72</v>
       </c>
       <c r="S9" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T9" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
@@ -3381,10 +3378,10 @@
         <v>30</v>
       </c>
       <c r="S10" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T10" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
@@ -3407,13 +3404,13 @@
     <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P13" s="46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q13" s="47"/>
       <c r="R13" s="47"/>
@@ -3427,27 +3424,27 @@
         <v>6</v>
       </c>
       <c r="K14" s="33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P14" s="25"/>
       <c r="Q14" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R14" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="T14" s="26"/>
     </row>
     <row r="15" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="P15" s="25"/>
       <c r="Q15" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R15" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S15" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T15" s="31">
         <v>64</v>
@@ -3455,16 +3452,16 @@
     </row>
     <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="P16" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q16" s="29">
         <v>8</v>
       </c>
       <c r="R16" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S16" s="27"/>
       <c r="T16" s="20" t="s">
@@ -3477,46 +3474,46 @@
         <v>300</v>
       </c>
       <c r="K17" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="9:17" x14ac:dyDescent="0.3">
       <c r="P18" s="51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q18" s="52"/>
     </row>
     <row r="19" spans="9:17" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P19" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q19" s="7" t="s">
         <v>112</v>
-      </c>
-      <c r="Q19" s="7" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="20" spans="9:17" x14ac:dyDescent="0.3">
       <c r="P20" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q20" s="50" t="s">
         <v>114</v>
-      </c>
-      <c r="Q20" s="50" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="21" spans="9:17" x14ac:dyDescent="0.3">
       <c r="P21" s="40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q21" s="50"/>
     </row>
     <row r="22" spans="9:17" x14ac:dyDescent="0.3">
       <c r="I22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3525,10 +3522,10 @@
         <v>212.05750411731105</v>
       </c>
       <c r="K23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3537,18 +3534,18 @@
         <v>70.685834705770347</v>
       </c>
       <c r="K24" s="33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3557,19 +3554,19 @@
         <v>706.85834705770344</v>
       </c>
       <c r="K27" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="9:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="31" spans="9:17" x14ac:dyDescent="0.3">
       <c r="I31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J31" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K31" s="19"/>
     </row>
@@ -3579,24 +3576,24 @@
         <v>400</v>
       </c>
       <c r="K32" s="35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="10:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="10:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J35" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K35" s="33">
         <f>20*20</f>
         <v>400</v>
       </c>
       <c r="L35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="10:12" x14ac:dyDescent="0.3">
@@ -3609,7 +3606,7 @@
     </row>
     <row r="37" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K37">
         <f>K35*K36</f>
@@ -3645,8 +3642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529E1EE1-84BC-44E9-9DB6-5CF40692FF92}">
   <dimension ref="B2:AS60"/>
   <sheetViews>
-    <sheetView topLeftCell="F15" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AA54" sqref="AA54"/>
+    <sheetView tabSelected="1" topLeftCell="F15" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="T35" sqref="T35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3685,7 +3682,7 @@
         <v>38</v>
       </c>
       <c r="AI51" s="43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="3:35" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3832,7 +3829,7 @@
         <v>37</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
@@ -3863,7 +3860,7 @@
         <v>1</v>
       </c>
       <c r="I26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.3">
@@ -3891,7 +3888,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -3899,7 +3896,7 @@
         <v>34</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -3907,7 +3904,7 @@
         <v>36</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -3915,15 +3912,15 @@
         <v>38</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>